<commit_message>
Automation UI Fixes for 17.11.1_RC web
</commit_message>
<xml_diff>
--- a/Finflux Automation Excels/Client/4933-EI-DB-SAR-PartialPeriod-RECAL-COMP-MultiTranche-Disburse2ndTranche.xlsx
+++ b/Finflux Automation Excels/Client/4933-EI-DB-SAR-PartialPeriod-RECAL-COMP-MultiTranche-Disburse2ndTranche.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
@@ -534,7 +534,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,8 +599,8 @@
       <c r="E3" s="6">
         <v>421.87</v>
       </c>
-      <c r="F3" s="6">
-        <v>0</v>
+      <c r="F3">
+        <v>81.150000000000006</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>